<commit_message>
Updated for latest D365 version
</commit_message>
<xml_diff>
--- a/TC_NewPurchaseOrder/Main.rvl.xlsx
+++ b/TC_NewPurchaseOrder/Main.rvl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="169">
   <si>
     <t>NavBarDashboard</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>DfoPassWelcomeScreen</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="99">
+  <borders count="101">
     <border outline="false">
       <left/>
       <right/>
@@ -649,11 +652,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
@@ -754,6 +759,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="96" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="97" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="98" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="100" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="true"/>
@@ -1052,7 +1059,7 @@
     <outlinePr/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection activeCell="$A$1" sqref="$A$1:$A$1"/>
@@ -1248,203 +1255,231 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>115</v>
-      </c>
-      <c r="F16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" t="s">
-        <v>38</v>
-      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="1"/>
+      <c r="A17" s="100"/>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" t="s">
+        <v>168</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G18" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="1"/>
     </row>
     <row r="21">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="B21" t="s">
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
         <v>96</v>
       </c>
-      <c r="G21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="1"/>
+      <c r="G23" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="G24" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" t="s">
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="G25" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26">
@@ -1455,16 +1490,16 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="G26" t="s">
         <v>95</v>
@@ -1475,43 +1510,45 @@
         <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
         <v>47</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="B28" t="s">
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29">
@@ -1522,19 +1559,19 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="G29" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30">
@@ -1542,45 +1579,43 @@
         <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
         <v>47</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="G31" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32">
@@ -1591,19 +1626,19 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G32" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33">
@@ -1611,127 +1646,111 @@
         <v>93</v>
       </c>
       <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
         <v>2</v>
       </c>
-      <c r="C33" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" t="s">
         <v>25</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F34" t="s">
         <v>47</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="1"/>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" t="s">
+    <row r="35">
+      <c r="A35" s="1"/>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
         <v>10</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>82</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>87</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>27</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" t="s">
-        <v>93</v>
-      </c>
-      <c r="G35" t="s">
-        <v>93</v>
-      </c>
-    </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A36" s="88"/>
       <c r="B36" t="s">
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="F36" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="G36" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="A37" s="92"/>
       <c r="B37" t="s">
         <v>2</v>
       </c>
-      <c r="C37" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" t="s">
-        <v>93</v>
-      </c>
       <c r="E37" t="s">
-        <v>25</v>
+        <v>159</v>
       </c>
       <c r="F37" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="G37" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1"/>
+      <c r="A38" s="93"/>
       <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="F38" t="s">
         <v>27</v>
@@ -1741,126 +1760,102 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="88"/>
+      <c r="A39" s="1"/>
       <c r="B39" t="s">
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="G39" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="92"/>
-      <c r="B40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>159</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="61"/>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="62"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1"/>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" t="s">
         <v>27</v>
       </c>
-      <c r="G40" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="93"/>
-      <c r="B41" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s">
-        <v>161</v>
-      </c>
-      <c r="F41" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1"/>
-      <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="61"/>
-      <c r="B44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44" t="s">
-        <v>47</v>
-      </c>
       <c r="G44" t="s">
-        <v>141</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="62"/>
+      <c r="A45" s="1"/>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" t="s">
-        <v>93</v>
-      </c>
-      <c r="G46" t="s">
-        <v>93</v>
-      </c>
+      <c r="A46" s="1"/>
     </row>
     <row r="47">
       <c r="A47" s="1"/>
@@ -1868,76 +1863,88 @@
         <v>36</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="E47" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="G47" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1"/>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1"/>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1"/>
-      <c r="B50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" t="s">
-        <v>56</v>
-      </c>
-      <c r="E50" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" t="s">
-        <v>93</v>
-      </c>
-      <c r="G50" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" s="1"/>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
       </c>
       <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" t="s">
         <v>29</v>
-      </c>
-      <c r="F51" t="s">
-        <v>100</v>
-      </c>
-      <c r="G51" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1"/>
       <c r="B52" t="s">
-        <v>36</v>
-      </c>
-      <c r="C52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="F52" t="s">
         <v>100</v>
@@ -1955,108 +1962,69 @@
         <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="E54" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F54" t="s">
         <v>47</v>
       </c>
       <c r="G54" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1"/>
-      <c r="B55" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" t="s">
-        <v>100</v>
-      </c>
-      <c r="G55" t="s">
-        <v>29</v>
-      </c>
+      <c r="A55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H55" s="1"/>
     </row>
     <row r="56">
       <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
     </row>
     <row r="57">
       <c r="A57" s="1"/>
-      <c r="B57" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" t="s">
-        <v>92</v>
-      </c>
-      <c r="E57" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" t="s">
-        <v>47</v>
-      </c>
-      <c r="G57" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H58" s="1"/>
+      <c r="A58" s="1"/>
     </row>
     <row r="59">
       <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
     </row>
     <row r="60">
       <c r="A60" s="1"/>
     </row>
     <row r="61">
       <c r="A61" s="1"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="1"/>
     </row>
   </sheetData>
   <sheetProtection/>

</xml_diff>